<commit_message>
Fixes in the CoCoMo estimate
</commit_message>
<xml_diff>
--- a/CoCoMoHelper.xlsx
+++ b/CoCoMoHelper.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,14 +9,78 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Product Design</t>
+  </si>
+  <si>
+    <t>Detailed Design</t>
+  </si>
+  <si>
+    <t>Code &amp; Unit Tests</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Effort (Person-Months)</t>
+  </si>
+  <si>
+    <t>Labour cost (K$)</t>
+  </si>
+  <si>
+    <t>Running costs (K$)</t>
+  </si>
+  <si>
+    <t>Fixed costs (K$)</t>
+  </si>
+  <si>
+    <t>Duration (Months)</t>
+  </si>
+  <si>
+    <t>Integration &amp; Test</t>
+  </si>
+  <si>
+    <t>Total cost (K$)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -44,19 +108,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -98,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +210,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +418,217 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0.8</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>D3+E3*H3+F3</f>
+        <v>1.5350000000000001</v>
+      </c>
+      <c r="H3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.3</v>
+      </c>
+      <c r="D4">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>D4+E$3*H4+F4</f>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0.4</v>
+      </c>
+      <c r="D5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>D5+E3*H5+F5</f>
+        <v>3.3499999999999996</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>2.8</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6">
+        <f>(1.65+1.1) * 3</f>
+        <v>8.25</v>
+      </c>
+      <c r="G6">
+        <f>D6+E3*H6+F6</f>
+        <v>12.414999999999999</v>
+      </c>
+      <c r="H6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>0.3</v>
+      </c>
+      <c r="D7">
+        <v>1.6</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7">
+        <v>3.2</v>
+      </c>
+      <c r="G7">
+        <f>D7+E3*H7+F7</f>
+        <v>5.6400000000000006</v>
+      </c>
+      <c r="H7">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C4:C7)</f>
+        <v>1.5</v>
+      </c>
+      <c r="D8">
+        <f>SUM(D4:D7)</f>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F8">
+        <f>SUM(F4:F7)</f>
+        <v>11.45</v>
+      </c>
+      <c r="G8">
+        <f>SUM(G4:G7)</f>
+        <v>23.954999999999998</v>
+      </c>
+      <c r="H8">
+        <f>SUM(H4:H7)</f>
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f>C8+C3</f>
+        <v>1.6</v>
+      </c>
+      <c r="D9">
+        <f>D8+D3</f>
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <f>F8+F3</f>
+        <v>11.45</v>
+      </c>
+      <c r="G9">
+        <f>G8+G3</f>
+        <v>25.49</v>
+      </c>
+      <c r="H9">
+        <f>H8+H3</f>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:E7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>